<commit_message>
NEON harvester: use new variable lookup table
</commit_message>
<xml_diff>
--- a/NEON/NEONHarvester/settings/neon_variables_lookup_example.xlsx
+++ b/NEON/NEONHarvester/settings/neon_variables_lookup_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="97">
   <si>
     <t xml:space="preserve">ProductCode</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">CuahsiVariableName</t>
   </si>
   <si>
+    <t xml:space="preserve">GeneralCategory</t>
+  </si>
+  <si>
     <t xml:space="preserve">SampleMedium</t>
   </si>
   <si>
@@ -61,15 +64,6 @@
     <t xml:space="preserve">UnitsID</t>
   </si>
   <si>
-    <t xml:space="preserve">TimeUnitsName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeUnitsID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeSupport</t>
-  </si>
-  <si>
     <t xml:space="preserve">DP1.00001.001</t>
   </si>
   <si>
@@ -85,15 +79,21 @@
     <t xml:space="preserve">windSpeedMean</t>
   </si>
   <si>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.00001.001</t>
+  </si>
+  <si>
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">windSpeedMean_2DWSD_30min_00001_001</t>
+    <t xml:space="preserve">DP1.00001.001_windSpeedMean</t>
   </si>
   <si>
     <t xml:space="preserve">Wind speed</t>
   </si>
   <si>
+    <t xml:space="preserve">Climate</t>
+  </si>
+  <si>
     <t xml:space="preserve">Air</t>
   </si>
   <si>
@@ -103,13 +103,10 @@
     <t xml:space="preserve">meters per second</t>
   </si>
   <si>
-    <t xml:space="preserve">minute</t>
-  </si>
-  <si>
     <t xml:space="preserve">windDirMean</t>
   </si>
   <si>
-    <t xml:space="preserve">windDirMean_2DWSD_30min_00001_001</t>
+    <t xml:space="preserve">DP1.00001.001_windDirMean</t>
   </si>
   <si>
     <t xml:space="preserve">Wind direction</t>
@@ -130,7 +127,10 @@
     <t xml:space="preserve">tempSingleMean</t>
   </si>
   <si>
-    <t xml:space="preserve">tempSingleMean_2DWSD_30min_00002_001</t>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.00002.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00002.001_tempSingleMean</t>
   </si>
   <si>
     <t xml:space="preserve">Temperature</t>
@@ -151,7 +151,10 @@
     <t xml:space="preserve">tempTripleMean</t>
   </si>
   <si>
-    <t xml:space="preserve">tempTripleMean_TAAT_30min_00003_001</t>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.00003.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00003.001_tempTripleMean</t>
   </si>
   <si>
     <t xml:space="preserve">DP1.00004.001</t>
@@ -166,7 +169,10 @@
     <t xml:space="preserve">staPresMean</t>
   </si>
   <si>
-    <t xml:space="preserve">staPresMean_BP_30min_00004_001</t>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.00004.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00004.001_staPresMean</t>
   </si>
   <si>
     <t xml:space="preserve">Pressure, gauge</t>
@@ -178,7 +184,7 @@
     <t xml:space="preserve">corPresMean</t>
   </si>
   <si>
-    <t xml:space="preserve">corPresMean_BP_30min_00004_001</t>
+    <t xml:space="preserve">DP1.00004.001_corPresMean</t>
   </si>
   <si>
     <t xml:space="preserve">DP1.00005.001</t>
@@ -217,7 +223,10 @@
     <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000898_DRAFT</t>
   </si>
   <si>
-    <t xml:space="preserve">priPrecipBulk_PRIPRE_30min_00006_001</t>
+    <t xml:space="preserve">DP1.00006.001_priPrecipBulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">millimeter</t>
   </si>
   <si>
     <t xml:space="preserve">SECPRE_30min</t>
@@ -229,7 +238,7 @@
     <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000816vA</t>
   </si>
   <si>
-    <t xml:space="preserve">secPrecipBulk_PRIPRE_30min_00006_001</t>
+    <t xml:space="preserve">DP1.00006.001_secPrecipBulk</t>
   </si>
   <si>
     <t xml:space="preserve">Paused</t>
@@ -409,10 +418,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -426,12 +435,11 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,125 +485,122 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="N2" s="1" t="n">
         <v>119</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>30</v>
-      </c>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="1" t="n">
+      <c r="N3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="P3" s="1" t="n">
-        <v>30</v>
-      </c>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>35</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>36</v>
@@ -604,25 +609,19 @@
         <v>37</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="1" t="n">
+      <c r="N4" s="1" t="n">
         <v>96</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="P4" s="1" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,7 +632,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>41</v>
@@ -641,397 +640,400 @@
       <c r="E5" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>43</v>
+      </c>
       <c r="G5" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="1" t="n">
+      <c r="N5" s="1" t="n">
         <v>96</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="P5" s="1" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" s="1" t="n">
+      <c r="M6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="1" t="n">
         <v>170</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="P6" s="1" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="0" t="s">
+      <c r="J7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M7" s="1" t="n">
+      <c r="N7" s="1" t="n">
         <v>170</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="P7" s="1" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M8" s="1" t="n">
+      <c r="N8" s="1" t="n">
         <v>96</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="P8" s="1" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E9" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>61</v>
+      <c r="J9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F10" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>61</v>
+      <c r="N10" s="0" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="H11" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="0" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="M14" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="N14" s="0" t="n">
         <v>199</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="J15" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="L15" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N15" s="0" t="n">
         <v>33</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O15" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="P15" s="1" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1"/>
       <c r="G16" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NEON: sensor position lookup using the last month of each site-data product pair
</commit_message>
<xml_diff>
--- a/NEON/NEONHarvester/settings/neon_variables_lookup_example.xlsx
+++ b/NEON/NEONHarvester/settings/neon_variables_lookup_example.xlsx
@@ -268,7 +268,7 @@
     <t xml:space="preserve">3D wind attitude and motion reference </t>
   </si>
   <si>
-    <t xml:space="preserve">NEON.DP1.00013 </t>
+    <t xml:space="preserve">DP1.00013.001</t>
   </si>
   <si>
     <t xml:space="preserve">Wet deposition chemical analysis </t>
@@ -283,7 +283,7 @@
     <t xml:space="preserve">milligrams per liter</t>
   </si>
   <si>
-    <t xml:space="preserve">NEON.DP1.00014</t>
+    <t xml:space="preserve">DP1.00014.001</t>
   </si>
   <si>
     <t xml:space="preserve">Shortwave radiation (direct and diffuse pyranometer) </t>
@@ -301,13 +301,13 @@
     <t xml:space="preserve">gloRadMean_SRDDP_30min_00014_001</t>
   </si>
   <si>
-    <t xml:space="preserve">Global Radiation</t>
+    <t xml:space="preserve">Global radiation</t>
   </si>
   <si>
     <t xml:space="preserve">watts per square meter </t>
   </si>
   <si>
-    <t xml:space="preserve">NEON.DP1.00017</t>
+    <t xml:space="preserve">DP1.00017.001</t>
   </si>
   <si>
     <t xml:space="preserve">Dust and particulate size distribution </t>
@@ -420,8 +420,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
NEON harvester code refactoring and cleanup
</commit_message>
<xml_diff>
--- a/NEON/NEONHarvester/settings/neon_variables_lookup_example.xlsx
+++ b/NEON/NEONHarvester/settings/neon_variables_lookup_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="97">
   <si>
     <t xml:space="preserve">ProductCode</t>
   </si>
@@ -420,8 +420,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1005,6 +1005,9 @@
       <c r="I15" s="0" t="s">
         <v>93</v>
       </c>
+      <c r="J15" s="0" t="s">
+        <v>23</v>
+      </c>
       <c r="K15" s="0" t="s">
         <v>24</v>
       </c>

</xml_diff>